<commit_message>
Restructuring and Renaming Files
</commit_message>
<xml_diff>
--- a/.Files/MPD.xlsx
+++ b/.Files/MPD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jowjokiyolo\Documents\MaintenanceECOFly\.Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9991C3-A2B9-4267-BFE5-6C1B548A51A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984E26E2-154D-47AD-9218-C90B0C3D1C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="5790" windowWidth="14400" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="5670" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14491,6 +14491,44 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -14518,44 +14556,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -14570,18 +14570,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{42C9C461-EB67-4FA3-8DD4-B93861E355AC}" name="Table1" displayName="Table1" ref="A1:I1678" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="9" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{42C9C461-EB67-4FA3-8DD4-B93861E355AC}" name="Table1" displayName="Table1" ref="A1:I1678" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7">
   <autoFilter ref="A1:I1678" xr:uid="{42C9C461-EB67-4FA3-8DD4-B93861E355AC}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{0345E1DF-4B41-40B8-BAEB-5EB197BBB01D}" name="Task Number"/>
-    <tableColumn id="2" xr3:uid="{1358AE62-72E4-4867-8264-600B62596BF3}" name="Zone" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{46E868D6-B9EF-47C7-999D-34E32371FB74}" name="Description" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{3DFF7AA1-115D-49B2-B4FC-80FED4551227}" name="Interval" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{F9A5E3A2-5650-4FD3-9EC4-1B7358E802E6}" name="MRB" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{C9598D29-D274-4B23-967E-7A9030291A89}" name="Reference" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{1358AE62-72E4-4867-8264-600B62596BF3}" name="Zone" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{46E868D6-B9EF-47C7-999D-34E32371FB74}" name="Description" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{3DFF7AA1-115D-49B2-B4FC-80FED4551227}" name="Interval" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{F9A5E3A2-5650-4FD3-9EC4-1B7358E802E6}" name="MRB" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{C9598D29-D274-4B23-967E-7A9030291A89}" name="Reference" dataDxfId="2"/>
     <tableColumn id="7" xr3:uid="{9690EDDA-7711-49E6-928F-6AFEF1DF491D}" name="Men"/>
-    <tableColumn id="8" xr3:uid="{BCD53127-D1A1-4651-9C9E-7EF2F37ECAD0}" name="M/H" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{6263A5EA-94BA-4059-A97E-61FFB9E0835B}" name="Effectivity" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{BCD53127-D1A1-4651-9C9E-7EF2F37ECAD0}" name="M/H" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{6263A5EA-94BA-4059-A97E-61FFB9E0835B}" name="Effectivity" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -14875,7 +14875,7 @@
   <dimension ref="A1:I1678"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34649,7 +34649,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="690" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="690" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A690" t="s">
         <v>2206</v>
       </c>
@@ -37798,7 +37798,7 @@
         <v>2542</v>
       </c>
     </row>
-    <row r="799" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="799" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A799" t="s">
         <v>2543</v>
       </c>
@@ -38256,7 +38256,7 @@
         <v>2563</v>
       </c>
     </row>
-    <row r="815" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="815" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A815" t="s">
         <v>2600</v>
       </c>
@@ -41255,7 +41255,7 @@
         <v>2897</v>
       </c>
     </row>
-    <row r="921" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="921" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A921" t="s">
         <v>2898</v>
       </c>
@@ -42925,7 +42925,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="979" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="979" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A979" t="s">
         <v>3037</v>
       </c>
@@ -61855,6 +61855,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="ef9a9971-8f81-456e-9573-47180d38c8d8" xsi:nil="true"/>
@@ -61863,15 +61872,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -62136,20 +62136,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0962F618-D14D-4399-B14C-CB2F094520C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EB3A98C-6CA3-428F-B5C9-01EB80BF13E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="ef9a9971-8f81-456e-9573-47180d38c8d8"/>
     <ds:schemaRef ds:uri="6b90f42b-64c4-4e1d-b8a2-9a34aba7b617"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0962F618-D14D-4399-B14C-CB2F094520C4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>